<commit_message>
MVC Learning + Logs
</commit_message>
<xml_diff>
--- a/Logs/4th Week Logs.xlsx
+++ b/Logs/4th Week Logs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE1950F-ED76-4071-91C6-A64EF7CABB2B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD9B34E-E266-400C-98EA-631AAE023AB9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -843,7 +843,7 @@
   <dimension ref="B2:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,14 +1079,28 @@
       <c r="K12" s="43"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="40"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
+      <c r="B13" s="40">
+        <v>6</v>
+      </c>
+      <c r="C13" s="8">
+        <v>43521</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="46"/>
+      <c r="G13" s="14">
+        <v>165</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="46" t="s">
+        <v>18</v>
+      </c>
       <c r="J13" s="4"/>
       <c r="K13" s="43"/>
     </row>
@@ -1172,7 +1186,7 @@
       </c>
       <c r="G20" s="20">
         <f>SUM(G8:G19)</f>
-        <v>635</v>
+        <v>800</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>

</xml_diff>